<commit_message>
Revert "gh v5 gh01"
This reverts commit 3554827977a2df478457e906888161365b23c7b4.
</commit_message>
<xml_diff>
--- a/excelv5.xlsx
+++ b/excelv5.xlsx
@@ -16,9 +16,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>gh01</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>aaaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>github for win2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wn3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbb</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -363,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -374,6 +394,31 @@
     <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "gh v5 gh01""
This reverts commit e7bf49f31a70e9b3319581f4f118d0759790975c.
</commit_message>
<xml_diff>
--- a/excelv5.xlsx
+++ b/excelv5.xlsx
@@ -16,29 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>aaaa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbbb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dddd</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>github for win2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wn3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbb</t>
+    <t>gh01</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -383,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B7"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -394,31 +374,6 @@
     <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>